<commit_message>
time and rm of dev env
</commit_message>
<xml_diff>
--- a/IP_Controlling_Bruno_Maikoff.xlsx
+++ b/IP_Controlling_Bruno_Maikoff.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\FHNW\Semester7\Bachlorthesis\BlockChain_TransactionManager\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspaces\BlockChain_TransactionManager\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBDF810E-22A2-4583-986A-60E94959F6E7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{242EB56A-3299-4313-ACFE-02C0B909EA25}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Arbeitsrapport_Bruno" sheetId="11" r:id="rId1"/>
@@ -564,8 +564,8 @@
     </xf>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Link" xfId="1" builtinId="8"/>
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Standard 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
   </cellStyles>
   <dxfs count="2">
@@ -680,7 +680,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="de-DE"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -998,7 +998,7 @@
                 <a:cs typeface="Arial"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1"/>
@@ -1053,7 +1053,7 @@
                 <a:cs typeface="Arial"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="2067145632"/>
@@ -1101,7 +1101,7 @@
           <a:cs typeface="Arial"/>
         </a:defRPr>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="de-DE"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1115,7 +1115,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="de-DE"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1313,70 +1313,70 @@
                   <c:v>63</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>63</c:v>
+                  <c:v>72</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>63</c:v>
+                  <c:v>72</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>63</c:v>
+                  <c:v>72</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>63</c:v>
+                  <c:v>72</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>63</c:v>
+                  <c:v>72</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>63</c:v>
+                  <c:v>72</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>63</c:v>
+                  <c:v>72</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>63</c:v>
+                  <c:v>72</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>63</c:v>
+                  <c:v>72</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>63</c:v>
+                  <c:v>72</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>63</c:v>
+                  <c:v>72</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>63</c:v>
+                  <c:v>72</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>63</c:v>
+                  <c:v>72</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>63</c:v>
+                  <c:v>72</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>63</c:v>
+                  <c:v>72</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>63</c:v>
+                  <c:v>72</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>63</c:v>
+                  <c:v>72</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>63</c:v>
+                  <c:v>72</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>63</c:v>
+                  <c:v>72</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>63</c:v>
+                  <c:v>72</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>63</c:v>
+                  <c:v>72</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>63</c:v>
+                  <c:v>72</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1433,7 +1433,7 @@
                 <a:cs typeface="Arial"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1"/>
@@ -1488,7 +1488,7 @@
                 <a:cs typeface="Arial"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="2067145632"/>
@@ -1536,7 +1536,7 @@
           <a:cs typeface="Arial"/>
         </a:defRPr>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="de-DE"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1983,22 +1983,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AG36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView topLeftCell="A4" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.59765625" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="8" customWidth="1"/>
-    <col min="2" max="2" width="10.28515625" customWidth="1"/>
-    <col min="3" max="3" width="10.28515625" style="15" customWidth="1"/>
-    <col min="4" max="4" width="9.42578125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="46.7109375" customWidth="1"/>
+    <col min="2" max="2" width="10.265625" customWidth="1"/>
+    <col min="3" max="3" width="10.265625" style="15" customWidth="1"/>
+    <col min="4" max="4" width="9.3984375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="46.73046875" customWidth="1"/>
     <col min="6" max="6" width="6" bestFit="1" customWidth="1"/>
-    <col min="7" max="33" width="4.7109375" customWidth="1"/>
+    <col min="7" max="33" width="4.73046875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" s="3" customFormat="1" ht="20.25" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:33" s="3" customFormat="1" ht="20.25" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="46" t="s">
         <v>3</v>
       </c>
@@ -2008,7 +2008,7 @@
       <c r="E1" s="46"/>
       <c r="F1" s="14"/>
     </row>
-    <row r="2" spans="1:33" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:33" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="47" t="s">
         <v>10</v>
       </c>
@@ -2103,7 +2103,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A3" s="47"/>
       <c r="B3" s="47"/>
       <c r="C3" s="47"/>
@@ -2220,7 +2220,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:33" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:33" ht="25.5" x14ac:dyDescent="0.35">
       <c r="A4" s="16" t="s">
         <v>5</v>
       </c>
@@ -2340,7 +2340,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="5" spans="1:33" s="8" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:33" s="8" customFormat="1" ht="26.25" x14ac:dyDescent="0.35">
       <c r="A5" s="17" t="s">
         <v>6</v>
       </c>
@@ -2468,7 +2468,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="6" spans="1:33" s="10" customFormat="1" ht="22.5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:33" s="10" customFormat="1" ht="20.25" x14ac:dyDescent="0.35">
       <c r="A6" s="22">
         <v>1</v>
       </c>
@@ -2487,7 +2487,7 @@
       </c>
       <c r="F6" s="9"/>
     </row>
-    <row r="7" spans="1:33" s="10" customFormat="1" ht="22.5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:33" s="10" customFormat="1" ht="20.25" x14ac:dyDescent="0.35">
       <c r="A7" s="22">
         <f t="shared" ref="A7:A22" si="33">A6+1</f>
         <v>2</v>
@@ -2508,7 +2508,7 @@
       </c>
       <c r="F7" s="9"/>
     </row>
-    <row r="8" spans="1:33" s="10" customFormat="1" ht="33.75" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:33" s="10" customFormat="1" ht="30.4" x14ac:dyDescent="0.35">
       <c r="A8" s="22">
         <f t="shared" si="33"/>
         <v>3</v>
@@ -2529,7 +2529,7 @@
       </c>
       <c r="F8" s="9"/>
     </row>
-    <row r="9" spans="1:33" s="10" customFormat="1" ht="22.5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:33" s="10" customFormat="1" ht="20.25" x14ac:dyDescent="0.35">
       <c r="A9" s="22">
         <f t="shared" si="33"/>
         <v>4</v>
@@ -2550,7 +2550,7 @@
       </c>
       <c r="F9" s="9"/>
     </row>
-    <row r="10" spans="1:33" s="11" customFormat="1" ht="22.5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:33" s="11" customFormat="1" ht="20.25" x14ac:dyDescent="0.35">
       <c r="A10" s="22">
         <f t="shared" si="33"/>
         <v>5</v>
@@ -2571,7 +2571,7 @@
       </c>
       <c r="F10" s="9"/>
     </row>
-    <row r="11" spans="1:33" s="11" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:33" s="11" customFormat="1" ht="10.15" x14ac:dyDescent="0.35">
       <c r="A11" s="22">
         <f t="shared" si="33"/>
         <v>6</v>
@@ -2592,7 +2592,7 @@
       </c>
       <c r="F11" s="9"/>
     </row>
-    <row r="12" spans="1:33" s="11" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:33" s="11" customFormat="1" ht="10.15" x14ac:dyDescent="0.35">
       <c r="A12" s="22">
         <f t="shared" si="33"/>
         <v>7</v>
@@ -2608,7 +2608,7 @@
       <c r="D12" s="31"/>
       <c r="E12" s="24"/>
     </row>
-    <row r="13" spans="1:33" s="11" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:33" s="11" customFormat="1" ht="10.15" x14ac:dyDescent="0.35">
       <c r="A13" s="22">
         <f t="shared" si="33"/>
         <v>8</v>
@@ -2624,7 +2624,7 @@
       <c r="D13" s="31"/>
       <c r="E13" s="24"/>
     </row>
-    <row r="14" spans="1:33" s="11" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:33" s="11" customFormat="1" ht="10.15" x14ac:dyDescent="0.35">
       <c r="A14" s="22">
         <f t="shared" si="33"/>
         <v>9</v>
@@ -2640,7 +2640,7 @@
       <c r="D14" s="31"/>
       <c r="E14" s="24"/>
     </row>
-    <row r="15" spans="1:33" s="11" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:33" s="11" customFormat="1" ht="10.15" x14ac:dyDescent="0.35">
       <c r="A15" s="22">
         <f t="shared" si="33"/>
         <v>10</v>
@@ -2656,7 +2656,7 @@
       <c r="D15" s="31"/>
       <c r="E15" s="24"/>
     </row>
-    <row r="16" spans="1:33" s="11" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:33" s="11" customFormat="1" ht="10.15" x14ac:dyDescent="0.35">
       <c r="A16" s="34">
         <f t="shared" si="33"/>
         <v>11</v>
@@ -2674,7 +2674,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="17" spans="1:5" s="11" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" s="11" customFormat="1" ht="10.15" x14ac:dyDescent="0.35">
       <c r="A17" s="38">
         <f t="shared" si="33"/>
         <v>12</v>
@@ -2689,7 +2689,7 @@
       </c>
       <c r="D17" s="31"/>
     </row>
-    <row r="18" spans="1:5" s="11" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" s="11" customFormat="1" ht="10.15" x14ac:dyDescent="0.35">
       <c r="A18" s="22">
         <f t="shared" si="33"/>
         <v>13</v>
@@ -2705,7 +2705,7 @@
       <c r="D18" s="31"/>
       <c r="E18" s="24"/>
     </row>
-    <row r="19" spans="1:5" s="11" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5" s="11" customFormat="1" ht="10.15" x14ac:dyDescent="0.35">
       <c r="A19" s="22">
         <f t="shared" si="33"/>
         <v>14</v>
@@ -2721,7 +2721,7 @@
       <c r="D19" s="31"/>
       <c r="E19" s="24"/>
     </row>
-    <row r="20" spans="1:5" s="11" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5" s="11" customFormat="1" ht="10.15" x14ac:dyDescent="0.35">
       <c r="A20" s="22">
         <f t="shared" si="33"/>
         <v>15</v>
@@ -2737,7 +2737,7 @@
       <c r="D20" s="31"/>
       <c r="E20" s="24"/>
     </row>
-    <row r="21" spans="1:5" s="11" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5" s="11" customFormat="1" ht="10.15" x14ac:dyDescent="0.35">
       <c r="A21" s="22">
         <f t="shared" si="33"/>
         <v>16</v>
@@ -2753,7 +2753,7 @@
       <c r="D21" s="31"/>
       <c r="E21" s="24"/>
     </row>
-    <row r="22" spans="1:5" s="11" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5" s="11" customFormat="1" ht="10.15" x14ac:dyDescent="0.35">
       <c r="A22" s="38">
         <f t="shared" si="33"/>
         <v>17</v>
@@ -2769,7 +2769,7 @@
       <c r="D22" s="31"/>
       <c r="E22" s="40"/>
     </row>
-    <row r="23" spans="1:5" s="11" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5" s="11" customFormat="1" ht="10.15" x14ac:dyDescent="0.35">
       <c r="A23" s="22">
         <v>18</v>
       </c>
@@ -2784,7 +2784,7 @@
       <c r="D23" s="31"/>
       <c r="E23" s="24"/>
     </row>
-    <row r="24" spans="1:5" s="11" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5" s="11" customFormat="1" ht="10.15" x14ac:dyDescent="0.35">
       <c r="A24" s="22">
         <v>19</v>
       </c>
@@ -2799,7 +2799,7 @@
       <c r="D24" s="31"/>
       <c r="E24" s="24"/>
     </row>
-    <row r="25" spans="1:5" s="11" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5" s="11" customFormat="1" ht="10.15" x14ac:dyDescent="0.35">
       <c r="A25" s="22">
         <v>20</v>
       </c>
@@ -2814,7 +2814,7 @@
       <c r="D25" s="31"/>
       <c r="E25" s="24"/>
     </row>
-    <row r="26" spans="1:5" s="11" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:5" s="11" customFormat="1" ht="10.15" x14ac:dyDescent="0.35">
       <c r="A26" s="22">
         <v>21</v>
       </c>
@@ -2829,7 +2829,7 @@
       <c r="D26" s="31"/>
       <c r="E26" s="24"/>
     </row>
-    <row r="27" spans="1:5" s="11" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:5" s="11" customFormat="1" ht="10.15" x14ac:dyDescent="0.35">
       <c r="A27" s="22">
         <v>22</v>
       </c>
@@ -2844,7 +2844,7 @@
       <c r="D27" s="31"/>
       <c r="E27" s="24"/>
     </row>
-    <row r="28" spans="1:5" s="11" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:5" s="11" customFormat="1" ht="10.15" x14ac:dyDescent="0.35">
       <c r="A28" s="22">
         <v>23</v>
       </c>
@@ -2859,7 +2859,7 @@
       <c r="D28" s="31"/>
       <c r="E28" s="24"/>
     </row>
-    <row r="29" spans="1:5" s="11" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:5" s="11" customFormat="1" ht="10.15" x14ac:dyDescent="0.35">
       <c r="A29" s="22">
         <v>24</v>
       </c>
@@ -2874,7 +2874,7 @@
       <c r="D29" s="31"/>
       <c r="E29" s="24"/>
     </row>
-    <row r="30" spans="1:5" s="11" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:5" s="11" customFormat="1" ht="10.15" x14ac:dyDescent="0.35">
       <c r="A30" s="22">
         <v>25</v>
       </c>
@@ -2889,7 +2889,7 @@
       <c r="D30" s="31"/>
       <c r="E30" s="24"/>
     </row>
-    <row r="31" spans="1:5" s="11" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:5" s="11" customFormat="1" ht="10.15" x14ac:dyDescent="0.35">
       <c r="A31" s="22">
         <v>26</v>
       </c>
@@ -2903,7 +2903,7 @@
       </c>
       <c r="D31" s="31"/>
     </row>
-    <row r="32" spans="1:5" s="11" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:5" s="11" customFormat="1" ht="10.15" x14ac:dyDescent="0.35">
       <c r="A32" s="34">
         <v>27</v>
       </c>
@@ -2920,14 +2920,14 @@
         <v>11</v>
       </c>
     </row>
-    <row r="33" spans="1:5" ht="6.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:5" ht="6.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33" s="25"/>
       <c r="B33" s="26"/>
       <c r="C33" s="26"/>
       <c r="D33" s="32"/>
       <c r="E33" s="27"/>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A34" s="50" t="s">
         <v>2</v>
       </c>
@@ -2939,14 +2939,14 @@
       </c>
       <c r="E34" s="12"/>
     </row>
-    <row r="35" spans="1:5" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A35" s="51"/>
       <c r="B35" s="51"/>
       <c r="C35" s="51"/>
       <c r="D35" s="51"/>
       <c r="E35" s="13"/>
     </row>
-    <row r="36" spans="1:5" ht="6.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:5" ht="6.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A36" s="25"/>
       <c r="B36" s="26"/>
       <c r="C36" s="26"/>
@@ -2976,22 +2976,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AG36"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="I34" sqref="I34"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="L37" sqref="L37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.59765625" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="8" customWidth="1"/>
-    <col min="2" max="2" width="10.28515625" customWidth="1"/>
-    <col min="3" max="3" width="10.28515625" style="15" customWidth="1"/>
-    <col min="4" max="4" width="9.42578125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="46.7109375" customWidth="1"/>
+    <col min="2" max="2" width="10.265625" customWidth="1"/>
+    <col min="3" max="3" width="10.265625" style="15" customWidth="1"/>
+    <col min="4" max="4" width="9.3984375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="46.73046875" customWidth="1"/>
     <col min="6" max="6" width="6" bestFit="1" customWidth="1"/>
-    <col min="7" max="33" width="4.7109375" customWidth="1"/>
+    <col min="7" max="33" width="4.73046875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" s="3" customFormat="1" ht="20.25" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:33" s="3" customFormat="1" ht="20.25" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="46" t="s">
         <v>3</v>
       </c>
@@ -3001,7 +3001,7 @@
       <c r="E1" s="46"/>
       <c r="F1" s="14"/>
     </row>
-    <row r="2" spans="1:33" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:33" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="47" t="s">
         <v>10</v>
       </c>
@@ -3096,7 +3096,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:33" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:33" ht="12.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="47"/>
       <c r="B3" s="47"/>
       <c r="C3" s="47"/>
@@ -3213,7 +3213,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:33" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:33" ht="25.5" x14ac:dyDescent="0.35">
       <c r="A4" s="43" t="s">
         <v>5</v>
       </c>
@@ -3333,7 +3333,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="5" spans="1:33" s="8" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:33" s="8" customFormat="1" ht="26.25" x14ac:dyDescent="0.35">
       <c r="A5" s="17" t="s">
         <v>6</v>
       </c>
@@ -3374,94 +3374,94 @@
       </c>
       <c r="L5" s="45">
         <f t="shared" si="2"/>
-        <v>63</v>
+        <v>72</v>
       </c>
       <c r="M5" s="45">
         <f t="shared" si="2"/>
-        <v>63</v>
+        <v>72</v>
       </c>
       <c r="N5" s="45">
         <f t="shared" si="2"/>
-        <v>63</v>
+        <v>72</v>
       </c>
       <c r="O5" s="45">
         <f t="shared" si="2"/>
-        <v>63</v>
+        <v>72</v>
       </c>
       <c r="P5" s="45">
         <f t="shared" si="2"/>
-        <v>63</v>
+        <v>72</v>
       </c>
       <c r="Q5" s="45">
         <f t="shared" si="2"/>
-        <v>63</v>
+        <v>72</v>
       </c>
       <c r="R5" s="45">
         <f t="shared" si="2"/>
-        <v>63</v>
+        <v>72</v>
       </c>
       <c r="S5" s="45">
         <f t="shared" si="2"/>
-        <v>63</v>
+        <v>72</v>
       </c>
       <c r="T5" s="45">
         <f t="shared" si="2"/>
-        <v>63</v>
+        <v>72</v>
       </c>
       <c r="U5" s="45">
         <f t="shared" si="2"/>
-        <v>63</v>
+        <v>72</v>
       </c>
       <c r="V5" s="45">
         <f t="shared" si="2"/>
-        <v>63</v>
+        <v>72</v>
       </c>
       <c r="W5" s="45">
         <f t="shared" si="2"/>
-        <v>63</v>
+        <v>72</v>
       </c>
       <c r="X5" s="45">
         <f t="shared" si="2"/>
-        <v>63</v>
+        <v>72</v>
       </c>
       <c r="Y5" s="45">
         <f t="shared" si="2"/>
-        <v>63</v>
+        <v>72</v>
       </c>
       <c r="Z5" s="45">
         <f t="shared" si="2"/>
-        <v>63</v>
+        <v>72</v>
       </c>
       <c r="AA5" s="45">
         <f t="shared" si="2"/>
-        <v>63</v>
+        <v>72</v>
       </c>
       <c r="AB5" s="45">
         <f t="shared" si="2"/>
-        <v>63</v>
+        <v>72</v>
       </c>
       <c r="AC5" s="45">
         <f t="shared" si="2"/>
-        <v>63</v>
+        <v>72</v>
       </c>
       <c r="AD5" s="45">
         <f t="shared" si="2"/>
-        <v>63</v>
+        <v>72</v>
       </c>
       <c r="AE5" s="45">
         <f t="shared" si="2"/>
-        <v>63</v>
+        <v>72</v>
       </c>
       <c r="AF5" s="45">
         <f t="shared" si="2"/>
-        <v>63</v>
+        <v>72</v>
       </c>
       <c r="AG5" s="45">
         <f t="shared" si="2"/>
-        <v>63</v>
-      </c>
-    </row>
-    <row r="6" spans="1:33" s="10" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="6" spans="1:33" s="10" customFormat="1" ht="10.15" x14ac:dyDescent="0.35">
       <c r="A6" s="22">
         <v>1</v>
       </c>
@@ -3480,7 +3480,7 @@
       </c>
       <c r="F6" s="9"/>
     </row>
-    <row r="7" spans="1:33" s="10" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:33" s="10" customFormat="1" ht="10.15" x14ac:dyDescent="0.35">
       <c r="A7" s="22">
         <f t="shared" ref="A7:A22" si="3">A6+1</f>
         <v>2</v>
@@ -3501,7 +3501,7 @@
       </c>
       <c r="F7" s="9"/>
     </row>
-    <row r="8" spans="1:33" s="10" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:33" s="10" customFormat="1" ht="10.15" x14ac:dyDescent="0.35">
       <c r="A8" s="22">
         <f t="shared" si="3"/>
         <v>3</v>
@@ -3522,7 +3522,7 @@
       </c>
       <c r="F8" s="9"/>
     </row>
-    <row r="9" spans="1:33" s="10" customFormat="1" ht="22.5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:33" s="10" customFormat="1" ht="20.25" x14ac:dyDescent="0.35">
       <c r="A9" s="22">
         <f t="shared" si="3"/>
         <v>4</v>
@@ -3543,7 +3543,7 @@
       </c>
       <c r="F9" s="9"/>
     </row>
-    <row r="10" spans="1:33" s="11" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:33" s="11" customFormat="1" ht="10.15" x14ac:dyDescent="0.35">
       <c r="A10" s="22">
         <f t="shared" si="3"/>
         <v>5</v>
@@ -3564,7 +3564,7 @@
       </c>
       <c r="F10" s="9"/>
     </row>
-    <row r="11" spans="1:33" s="11" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:33" s="11" customFormat="1" ht="10.15" x14ac:dyDescent="0.35">
       <c r="A11" s="22">
         <f t="shared" si="3"/>
         <v>6</v>
@@ -3577,11 +3577,13 @@
         <f t="shared" si="4"/>
         <v>43765</v>
       </c>
-      <c r="D11" s="31"/>
+      <c r="D11" s="31">
+        <v>9</v>
+      </c>
       <c r="E11" s="24"/>
       <c r="F11" s="9"/>
     </row>
-    <row r="12" spans="1:33" s="11" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:33" s="11" customFormat="1" ht="10.15" x14ac:dyDescent="0.35">
       <c r="A12" s="22">
         <f t="shared" si="3"/>
         <v>7</v>
@@ -3597,7 +3599,7 @@
       <c r="D12" s="31"/>
       <c r="E12" s="24"/>
     </row>
-    <row r="13" spans="1:33" s="11" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:33" s="11" customFormat="1" ht="10.15" x14ac:dyDescent="0.35">
       <c r="A13" s="22">
         <f t="shared" si="3"/>
         <v>8</v>
@@ -3613,7 +3615,7 @@
       <c r="D13" s="31"/>
       <c r="E13" s="24"/>
     </row>
-    <row r="14" spans="1:33" s="11" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:33" s="11" customFormat="1" ht="10.15" x14ac:dyDescent="0.35">
       <c r="A14" s="22">
         <f t="shared" si="3"/>
         <v>9</v>
@@ -3629,7 +3631,7 @@
       <c r="D14" s="31"/>
       <c r="E14" s="24"/>
     </row>
-    <row r="15" spans="1:33" s="11" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:33" s="11" customFormat="1" ht="10.15" x14ac:dyDescent="0.35">
       <c r="A15" s="22">
         <f t="shared" si="3"/>
         <v>10</v>
@@ -3645,7 +3647,7 @@
       <c r="D15" s="31"/>
       <c r="E15" s="24"/>
     </row>
-    <row r="16" spans="1:33" s="11" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:33" s="11" customFormat="1" ht="10.15" x14ac:dyDescent="0.35">
       <c r="A16" s="34">
         <f t="shared" si="3"/>
         <v>11</v>
@@ -3663,7 +3665,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="17" spans="1:5" s="11" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" s="11" customFormat="1" ht="10.15" x14ac:dyDescent="0.35">
       <c r="A17" s="38">
         <f t="shared" si="3"/>
         <v>12</v>
@@ -3678,7 +3680,7 @@
       </c>
       <c r="D17" s="31"/>
     </row>
-    <row r="18" spans="1:5" s="11" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" s="11" customFormat="1" ht="10.15" x14ac:dyDescent="0.35">
       <c r="A18" s="22">
         <f t="shared" si="3"/>
         <v>13</v>
@@ -3694,7 +3696,7 @@
       <c r="D18" s="31"/>
       <c r="E18" s="24"/>
     </row>
-    <row r="19" spans="1:5" s="11" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5" s="11" customFormat="1" ht="10.15" x14ac:dyDescent="0.35">
       <c r="A19" s="22">
         <f t="shared" si="3"/>
         <v>14</v>
@@ -3710,7 +3712,7 @@
       <c r="D19" s="31"/>
       <c r="E19" s="24"/>
     </row>
-    <row r="20" spans="1:5" s="11" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5" s="11" customFormat="1" ht="10.15" x14ac:dyDescent="0.35">
       <c r="A20" s="22">
         <f t="shared" si="3"/>
         <v>15</v>
@@ -3726,7 +3728,7 @@
       <c r="D20" s="31"/>
       <c r="E20" s="24"/>
     </row>
-    <row r="21" spans="1:5" s="11" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5" s="11" customFormat="1" ht="10.15" x14ac:dyDescent="0.35">
       <c r="A21" s="22">
         <f t="shared" si="3"/>
         <v>16</v>
@@ -3742,7 +3744,7 @@
       <c r="D21" s="31"/>
       <c r="E21" s="24"/>
     </row>
-    <row r="22" spans="1:5" s="11" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5" s="11" customFormat="1" ht="10.15" x14ac:dyDescent="0.35">
       <c r="A22" s="38">
         <f t="shared" si="3"/>
         <v>17</v>
@@ -3758,7 +3760,7 @@
       <c r="D22" s="31"/>
       <c r="E22" s="40"/>
     </row>
-    <row r="23" spans="1:5" s="11" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5" s="11" customFormat="1" ht="10.15" x14ac:dyDescent="0.35">
       <c r="A23" s="22">
         <v>18</v>
       </c>
@@ -3773,7 +3775,7 @@
       <c r="D23" s="31"/>
       <c r="E23" s="24"/>
     </row>
-    <row r="24" spans="1:5" s="11" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5" s="11" customFormat="1" ht="10.15" x14ac:dyDescent="0.35">
       <c r="A24" s="22">
         <v>19</v>
       </c>
@@ -3788,7 +3790,7 @@
       <c r="D24" s="31"/>
       <c r="E24" s="24"/>
     </row>
-    <row r="25" spans="1:5" s="11" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5" s="11" customFormat="1" ht="10.15" x14ac:dyDescent="0.35">
       <c r="A25" s="22">
         <v>20</v>
       </c>
@@ -3803,7 +3805,7 @@
       <c r="D25" s="31"/>
       <c r="E25" s="24"/>
     </row>
-    <row r="26" spans="1:5" s="11" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:5" s="11" customFormat="1" ht="10.15" x14ac:dyDescent="0.35">
       <c r="A26" s="22">
         <v>21</v>
       </c>
@@ -3818,7 +3820,7 @@
       <c r="D26" s="31"/>
       <c r="E26" s="24"/>
     </row>
-    <row r="27" spans="1:5" s="11" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:5" s="11" customFormat="1" ht="10.15" x14ac:dyDescent="0.35">
       <c r="A27" s="22">
         <v>22</v>
       </c>
@@ -3833,7 +3835,7 @@
       <c r="D27" s="31"/>
       <c r="E27" s="24"/>
     </row>
-    <row r="28" spans="1:5" s="11" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:5" s="11" customFormat="1" ht="10.15" x14ac:dyDescent="0.35">
       <c r="A28" s="22">
         <v>23</v>
       </c>
@@ -3848,7 +3850,7 @@
       <c r="D28" s="31"/>
       <c r="E28" s="24"/>
     </row>
-    <row r="29" spans="1:5" s="11" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:5" s="11" customFormat="1" ht="10.15" x14ac:dyDescent="0.35">
       <c r="A29" s="22">
         <v>24</v>
       </c>
@@ -3863,7 +3865,7 @@
       <c r="D29" s="31"/>
       <c r="E29" s="24"/>
     </row>
-    <row r="30" spans="1:5" s="11" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:5" s="11" customFormat="1" ht="10.15" x14ac:dyDescent="0.35">
       <c r="A30" s="22">
         <v>25</v>
       </c>
@@ -3878,7 +3880,7 @@
       <c r="D30" s="31"/>
       <c r="E30" s="24"/>
     </row>
-    <row r="31" spans="1:5" s="11" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:5" s="11" customFormat="1" ht="10.15" x14ac:dyDescent="0.35">
       <c r="A31" s="22">
         <v>26</v>
       </c>
@@ -3892,7 +3894,7 @@
       </c>
       <c r="D31" s="31"/>
     </row>
-    <row r="32" spans="1:5" s="11" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:5" s="11" customFormat="1" ht="10.15" x14ac:dyDescent="0.35">
       <c r="A32" s="34">
         <v>27</v>
       </c>
@@ -3909,14 +3911,14 @@
         <v>11</v>
       </c>
     </row>
-    <row r="33" spans="1:5" ht="6.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:5" ht="6.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33" s="25"/>
       <c r="B33" s="26"/>
       <c r="C33" s="26"/>
       <c r="D33" s="32"/>
       <c r="E33" s="27"/>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A34" s="50" t="s">
         <v>2</v>
       </c>
@@ -3924,18 +3926,18 @@
       <c r="C34" s="50"/>
       <c r="D34" s="33">
         <f>SUM(D6:D33)</f>
-        <v>63</v>
+        <v>72</v>
       </c>
       <c r="E34" s="12"/>
     </row>
-    <row r="35" spans="1:5" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A35" s="51"/>
       <c r="B35" s="51"/>
       <c r="C35" s="51"/>
       <c r="D35" s="51"/>
       <c r="E35" s="13"/>
     </row>
-    <row r="36" spans="1:5" ht="6.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:5" ht="6.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A36" s="25"/>
       <c r="B36" s="26"/>
       <c r="C36" s="26"/>

</xml_diff>

<commit_message>
Report für diese Woche
</commit_message>
<xml_diff>
--- a/IP_Controlling_Bruno_Maikoff.xlsx
+++ b/IP_Controlling_Bruno_Maikoff.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\workspace\BlockChain_TransactionManager\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\FHNW\Semester7\Bachlorthesis\BlockChain_TransactionManager\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB6AA5A1-6C99-4A62-A570-06234977B268}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EA2E947-4977-49F8-B3F8-8D2F752E0AAB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11265" yWindow="2145" windowWidth="38700" windowHeight="14790" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Arbeitsrapport_Bruno" sheetId="11" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="50">
   <si>
     <t>Aufwand in h</t>
   </si>
@@ -187,6 +187,9 @@
   </si>
   <si>
     <t>Raport korrigiert, Algo weiter, Tests, Java fehler korrigiert, Manuelle tests, Abnahmekriterien, testreport</t>
+  </si>
+  <si>
+    <t>Programm, Report, Statusmeeting; Deployable, Tests</t>
   </si>
 </sst>
 </file>
@@ -1000,19 +1003,19 @@
                   <c:v>217</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>241</c:v>
+                  <c:v>249</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>241</c:v>
+                  <c:v>279</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>241</c:v>
+                  <c:v>279</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>241</c:v>
+                  <c:v>279</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>241</c:v>
+                  <c:v>279</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2054,8 +2057,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AG36"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AD5" sqref="AD5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2520,23 +2523,23 @@
       </c>
       <c r="AC5" s="45">
         <f t="shared" si="29"/>
-        <v>241</v>
+        <v>249</v>
       </c>
       <c r="AD5" s="45">
         <f t="shared" si="29"/>
-        <v>241</v>
+        <v>279</v>
       </c>
       <c r="AE5" s="45">
         <f t="shared" ref="AE5" si="30">AD5+SUMIF($A$6:$A$33,AE3,$D$6:$D$33)</f>
-        <v>241</v>
+        <v>279</v>
       </c>
       <c r="AF5" s="45">
         <f t="shared" ref="AF5" si="31">AE5+SUMIF($A$6:$A$33,AF3,$D$6:$D$33)</f>
-        <v>241</v>
+        <v>279</v>
       </c>
       <c r="AG5" s="45">
         <f t="shared" ref="AG5" si="32">AF5+SUMIF($A$6:$A$33,AG3,$D$6:$D$33)</f>
-        <v>241</v>
+        <v>279</v>
       </c>
     </row>
     <row r="6" spans="1:33" s="10" customFormat="1" ht="22.5" x14ac:dyDescent="0.2">
@@ -2975,7 +2978,7 @@
         <v>43884</v>
       </c>
       <c r="D28" s="31">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="E28" s="24" t="s">
         <v>48</v>
@@ -2993,8 +2996,12 @@
         <f t="shared" si="35"/>
         <v>43891</v>
       </c>
-      <c r="D29" s="31"/>
-      <c r="E29" s="24"/>
+      <c r="D29" s="31">
+        <v>30</v>
+      </c>
+      <c r="E29" s="24" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="30" spans="1:5" s="11" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A30" s="22">
@@ -3057,7 +3064,7 @@
       <c r="C34" s="50"/>
       <c r="D34" s="33">
         <f>SUM(D6:D33)</f>
-        <v>241</v>
+        <v>279</v>
       </c>
       <c r="E34" s="12"/>
     </row>
@@ -3098,8 +3105,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AG36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="M34" sqref="M34"/>
+    <sheetView topLeftCell="A19" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
proof reading, time logging
</commit_message>
<xml_diff>
--- a/IP_Controlling_Bruno_Maikoff.xlsx
+++ b/IP_Controlling_Bruno_Maikoff.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\workspace\BlockChain_TransactionManager\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{950794EB-F358-4E77-8A2F-C85D5116F923}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97F501E2-28A8-4DD4-8114-2EAD0E3BA1F9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="11265" yWindow="2145" windowWidth="38700" windowHeight="14790" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -75,9 +75,6 @@
     <t>Vorname, Name:</t>
   </si>
   <si>
-    <t xml:space="preserve"> Abgabe</t>
-  </si>
-  <si>
     <t>Sergejurij, Maikoff</t>
   </si>
   <si>
@@ -202,6 +199,9 @@
   </si>
   <si>
     <t>Testing, Java, AK, Betriebshandbuch</t>
+  </si>
+  <si>
+    <t>Report, Abgabe</t>
   </si>
 </sst>
 </file>
@@ -1462,7 +1462,7 @@
                   <c:v>412</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>412</c:v>
+                  <c:v>427</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2101,7 +2101,7 @@
       <c r="B2" s="47"/>
       <c r="C2" s="47"/>
       <c r="D2" s="48" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E2" s="49"/>
       <c r="F2" s="14" t="s">
@@ -2569,7 +2569,7 @@
         <v>4</v>
       </c>
       <c r="E6" s="24" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F6" s="9"/>
     </row>
@@ -2590,7 +2590,7 @@
         <v>6</v>
       </c>
       <c r="E7" s="24" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F7" s="9"/>
     </row>
@@ -2611,7 +2611,7 @@
         <v>10</v>
       </c>
       <c r="E8" s="24" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F8" s="9"/>
     </row>
@@ -2632,7 +2632,7 @@
         <v>12</v>
       </c>
       <c r="E9" s="24" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F9" s="9"/>
     </row>
@@ -2653,7 +2653,7 @@
         <v>11</v>
       </c>
       <c r="E10" s="24" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F10" s="9"/>
     </row>
@@ -2674,7 +2674,7 @@
         <v>9</v>
       </c>
       <c r="E11" s="24" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F11" s="9"/>
     </row>
@@ -2712,7 +2712,7 @@
         <v>7</v>
       </c>
       <c r="E13" s="24" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="14" spans="1:33" s="11" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
@@ -2732,7 +2732,7 @@
         <v>12</v>
       </c>
       <c r="E14" s="24" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="15" spans="1:33" s="11" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
@@ -2752,7 +2752,7 @@
         <v>18</v>
       </c>
       <c r="E15" s="24" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="16" spans="1:33" s="11" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
@@ -2772,7 +2772,7 @@
         <v>15</v>
       </c>
       <c r="E16" s="37" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="17" spans="1:5" s="11" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
@@ -2825,7 +2825,7 @@
         <v>10</v>
       </c>
       <c r="E19" s="24" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="20" spans="1:5" s="11" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
@@ -2845,7 +2845,7 @@
         <v>4</v>
       </c>
       <c r="E20" s="24" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="21" spans="1:5" s="11" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
@@ -2881,7 +2881,7 @@
         <v>5</v>
       </c>
       <c r="E22" s="40" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="23" spans="1:5" s="11" customFormat="1" ht="33.75" x14ac:dyDescent="0.2">
@@ -2900,7 +2900,7 @@
         <v>16</v>
       </c>
       <c r="E23" s="24" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="24" spans="1:5" s="11" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
@@ -2919,7 +2919,7 @@
         <v>16</v>
       </c>
       <c r="E24" s="24" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="25" spans="1:5" s="11" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
@@ -2955,7 +2955,7 @@
         <v>24</v>
       </c>
       <c r="E26" s="24" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="27" spans="1:5" s="11" customFormat="1" ht="22.5" x14ac:dyDescent="0.2">
@@ -2974,7 +2974,7 @@
         <v>26</v>
       </c>
       <c r="E27" s="24" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="28" spans="1:5" s="11" customFormat="1" ht="22.5" x14ac:dyDescent="0.2">
@@ -2993,7 +2993,7 @@
         <v>32</v>
       </c>
       <c r="E28" s="24" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="29" spans="1:5" s="11" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
@@ -3012,7 +3012,7 @@
         <v>22</v>
       </c>
       <c r="E29" s="24" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="30" spans="1:5" s="11" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
@@ -3031,7 +3031,7 @@
         <v>51</v>
       </c>
       <c r="E30" s="24" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="31" spans="1:5" s="11" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
@@ -3050,7 +3050,7 @@
         <v>46</v>
       </c>
       <c r="E31" s="11" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="32" spans="1:5" s="11" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
@@ -3067,7 +3067,7 @@
       </c>
       <c r="D32" s="36"/>
       <c r="E32" s="37" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="6.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3127,7 +3127,7 @@
   <dimension ref="A1:AG36"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="E44" sqref="E44"/>
+      <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3158,7 +3158,7 @@
       <c r="B2" s="47"/>
       <c r="C2" s="47"/>
       <c r="D2" s="48" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E2" s="49"/>
       <c r="F2" s="14" t="s">
@@ -3608,7 +3608,7 @@
       </c>
       <c r="AG5" s="45">
         <f t="shared" si="2"/>
-        <v>412</v>
+        <v>427</v>
       </c>
     </row>
     <row r="6" spans="1:33" s="10" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
@@ -3626,7 +3626,7 @@
         <v>3</v>
       </c>
       <c r="E6" s="24" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F6" s="9"/>
     </row>
@@ -3647,7 +3647,7 @@
         <v>6</v>
       </c>
       <c r="E7" s="24" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F7" s="9"/>
     </row>
@@ -3668,7 +3668,7 @@
         <v>22</v>
       </c>
       <c r="E8" s="24" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F8" s="9"/>
     </row>
@@ -3689,7 +3689,7 @@
         <v>18</v>
       </c>
       <c r="E9" s="24" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F9" s="9"/>
     </row>
@@ -3710,7 +3710,7 @@
         <v>14</v>
       </c>
       <c r="E10" s="24" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F10" s="9"/>
     </row>
@@ -3731,7 +3731,7 @@
         <v>12</v>
       </c>
       <c r="E11" s="24" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F11" s="9"/>
     </row>
@@ -3752,7 +3752,7 @@
         <v>9</v>
       </c>
       <c r="E12" s="24" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="13" spans="1:33" s="11" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
@@ -3772,7 +3772,7 @@
         <v>13</v>
       </c>
       <c r="E13" s="24" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="14" spans="1:33" s="11" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
@@ -3792,7 +3792,7 @@
         <v>8</v>
       </c>
       <c r="E14" s="24" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="15" spans="1:33" s="11" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
@@ -3812,7 +3812,7 @@
         <v>13</v>
       </c>
       <c r="E15" s="24" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="16" spans="1:33" s="11" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
@@ -3832,7 +3832,7 @@
         <v>7</v>
       </c>
       <c r="E16" s="37" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="17" spans="1:5" s="11" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
@@ -3852,7 +3852,7 @@
         <v>9</v>
       </c>
       <c r="E17" s="11" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="18" spans="1:5" s="11" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
@@ -3872,7 +3872,7 @@
         <v>16</v>
       </c>
       <c r="E18" s="24" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="19" spans="1:5" s="11" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
@@ -3892,7 +3892,7 @@
         <v>10</v>
       </c>
       <c r="E19" s="24" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="20" spans="1:5" s="11" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
@@ -3930,7 +3930,7 @@
         <v>15</v>
       </c>
       <c r="E21" s="24" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="22" spans="1:5" s="11" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
@@ -3950,7 +3950,7 @@
         <v>8</v>
       </c>
       <c r="E22" s="40" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="23" spans="1:5" s="11" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
@@ -3969,7 +3969,7 @@
         <v>19</v>
       </c>
       <c r="E23" s="24" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="24" spans="1:5" s="11" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
@@ -3988,7 +3988,7 @@
         <v>16</v>
       </c>
       <c r="E24" s="24" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="25" spans="1:5" s="11" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
@@ -4007,7 +4007,7 @@
         <v>12</v>
       </c>
       <c r="E25" s="24" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="26" spans="1:5" s="11" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
@@ -4026,7 +4026,7 @@
         <v>17</v>
       </c>
       <c r="E26" s="24" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="27" spans="1:5" s="11" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
@@ -4045,7 +4045,7 @@
         <v>20</v>
       </c>
       <c r="E27" s="24" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="28" spans="1:5" s="11" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
@@ -4064,7 +4064,7 @@
         <v>30</v>
       </c>
       <c r="E28" s="24" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="29" spans="1:5" s="11" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
@@ -4083,7 +4083,7 @@
         <v>33</v>
       </c>
       <c r="E29" s="24" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="30" spans="1:5" s="11" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
@@ -4102,7 +4102,7 @@
         <v>42</v>
       </c>
       <c r="E30" s="24" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="31" spans="1:5" s="11" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
@@ -4121,7 +4121,7 @@
         <v>40</v>
       </c>
       <c r="E31" s="11" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="32" spans="1:5" s="11" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
@@ -4136,9 +4136,11 @@
         <f>C31+5</f>
         <v>43910</v>
       </c>
-      <c r="D32" s="36"/>
+      <c r="D32" s="36">
+        <v>15</v>
+      </c>
       <c r="E32" s="37" t="s">
-        <v>11</v>
+        <v>53</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="6.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4156,7 +4158,7 @@
       <c r="C34" s="50"/>
       <c r="D34" s="33">
         <f>SUM(D6:D33)</f>
-        <v>412</v>
+        <v>427</v>
       </c>
       <c r="E34" s="12"/>
     </row>

</xml_diff>